<commit_message>
Se sube de nuevo casos de prueba
</commit_message>
<xml_diff>
--- a/Documentos proyecto San Ambiente/Fase2/Casos de Prueba/Casos de prueba plantilla.xlsx
+++ b/Documentos proyecto San Ambiente/Fase2/Casos de Prueba/Casos de prueba plantilla.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SanAmbiente\Proyecto-Sanambiente\Documentos proyecto San Ambiente\Fase2\Casos de Prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FCFD8B-C114-4928-903B-B5791292AB1D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BC60CD-8F24-46F7-A882-1F77E0548FA3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -2109,6 +2109,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2181,9 +2196,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2195,18 +2207,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2560,214 +2560,214 @@
   <sheetData>
     <row r="5" spans="2:13" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="40" t="s">
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="42"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="47"/>
     </row>
     <row r="7" spans="2:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="34"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="44"/>
-      <c r="M7" s="45"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="50"/>
     </row>
     <row r="8" spans="2:13" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="37"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="48"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="53"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="55" t="s">
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="55"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="55"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="52"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="55"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="55"/>
-      <c r="L11" s="55"/>
-      <c r="M11" s="55"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
     </row>
     <row r="12" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="61"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="55"/>
-      <c r="M12" s="55"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
     </row>
     <row r="13" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="55"/>
-      <c r="L13" s="55"/>
-      <c r="M13" s="55"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
     </row>
     <row r="14" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="57"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="61"/>
       <c r="F14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="58"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="55"/>
-      <c r="M14" s="55"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
     </row>
     <row r="15" spans="2:13" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="55" t="s">
+      <c r="C15" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="55" t="s">
+      <c r="D15" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="60" t="s">
+      <c r="E15" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="60" t="s">
+      <c r="F15" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="60" t="s">
+      <c r="G15" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="H15" s="60" t="s">
+      <c r="H15" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="I15" s="55" t="s">
+      <c r="I15" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="J15" s="55" t="s">
+      <c r="J15" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="K15" s="55" t="s">
+      <c r="K15" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="L15" s="55" t="s">
+      <c r="L15" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="55" t="s">
+      <c r="M15" s="31" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="55"/>
-      <c r="L16" s="55"/>
-      <c r="M16" s="55"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
     </row>
     <row r="17" spans="2:13" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="55"/>
-      <c r="L17" s="55"/>
-      <c r="M17" s="55"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
@@ -2897,6 +2897,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B6:H8"/>
+    <mergeCell ref="I6:M8"/>
+    <mergeCell ref="B9:H10"/>
+    <mergeCell ref="I9:M14"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="F15:F17"/>
     <mergeCell ref="L15:L17"/>
     <mergeCell ref="M15:M17"/>
     <mergeCell ref="C11:H11"/>
@@ -2907,17 +2918,6 @@
     <mergeCell ref="I15:I17"/>
     <mergeCell ref="J15:J17"/>
     <mergeCell ref="K15:K17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="B6:H8"/>
-    <mergeCell ref="I6:M8"/>
-    <mergeCell ref="B9:H10"/>
-    <mergeCell ref="I9:M14"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="G14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2950,50 +2950,50 @@
   <sheetData>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="40" t="s">
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="42"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="47"/>
     </row>
     <row r="5" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="34"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="45"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="50"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="48"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="53"/>
     </row>
     <row r="7" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
@@ -3056,18 +3056,18 @@
         <v>12</v>
       </c>
       <c r="C10" s="79"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="57"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="61"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="58"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="54"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="59"/>
     </row>
     <row r="11" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="64" t="s">
@@ -3345,11 +3345,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="J11:J13"/>
-    <mergeCell ref="K11:K13"/>
-    <mergeCell ref="L11:L13"/>
-    <mergeCell ref="M11:M13"/>
-    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
     <mergeCell ref="B4:H6"/>
     <mergeCell ref="I4:M6"/>
     <mergeCell ref="I7:M10"/>
@@ -3358,12 +3358,12 @@
     <mergeCell ref="C9:H9"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="G10:H10"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="L11:L13"/>
+    <mergeCell ref="M11:M13"/>
+    <mergeCell ref="G11:G13"/>
     <mergeCell ref="H11:H13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
     <mergeCell ref="I11:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3398,50 +3398,50 @@
   <sheetData>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="40" t="s">
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="42"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="47"/>
     </row>
     <row r="5" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="34"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="45"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="50"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="48"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="53"/>
     </row>
     <row r="7" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
@@ -3504,18 +3504,18 @@
         <v>12</v>
       </c>
       <c r="C10" s="79"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="57"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="61"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="58"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="54"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="59"/>
     </row>
     <row r="11" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="64" t="s">
@@ -3793,14 +3793,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B4:H6"/>
-    <mergeCell ref="I4:M6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="I7:M10"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="G10:H10"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
@@ -3813,6 +3805,14 @@
     <mergeCell ref="J11:J13"/>
     <mergeCell ref="K11:K13"/>
     <mergeCell ref="L11:L13"/>
+    <mergeCell ref="B4:H6"/>
+    <mergeCell ref="I4:M6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="I7:M10"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="G10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3823,8 +3823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF69378-5C9E-410A-9F24-6A5C43D39D40}">
   <dimension ref="B3:M21"/>
   <sheetViews>
-    <sheetView zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:H9"/>
+    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3844,50 +3844,50 @@
   <sheetData>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="40" t="s">
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="42"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="47"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="34"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="45"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="50"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="48"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="53"/>
     </row>
     <row r="7" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
@@ -3950,18 +3950,18 @@
         <v>12</v>
       </c>
       <c r="C10" s="79"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="57"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="61"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="58"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="54"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="59"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="64" t="s">
@@ -4239,14 +4239,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B4:H6"/>
-    <mergeCell ref="I4:M6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="I7:M10"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="G10:H10"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
@@ -4259,6 +4251,14 @@
     <mergeCell ref="J11:J13"/>
     <mergeCell ref="K11:K13"/>
     <mergeCell ref="L11:L13"/>
+    <mergeCell ref="B4:H6"/>
+    <mergeCell ref="I4:M6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="I7:M10"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="G10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -4269,7 +4269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E65285-BD75-4307-9A81-36792F3C310E}">
   <dimension ref="B3:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+    <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <selection activeCell="C9" sqref="C9:H9"/>
     </sheetView>
   </sheetViews>
@@ -4290,50 +4290,50 @@
   <sheetData>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="40" t="s">
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="42"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="47"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="34"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="45"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="50"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="48"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="53"/>
     </row>
     <row r="7" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
@@ -4396,18 +4396,18 @@
         <v>12</v>
       </c>
       <c r="C10" s="79"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="57"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="61"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="58"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="54"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="59"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="64" t="s">
@@ -4685,14 +4685,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B4:H6"/>
-    <mergeCell ref="I4:M6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="I7:M10"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="G10:H10"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
@@ -4705,6 +4697,14 @@
     <mergeCell ref="J11:J13"/>
     <mergeCell ref="K11:K13"/>
     <mergeCell ref="L11:L13"/>
+    <mergeCell ref="B4:H6"/>
+    <mergeCell ref="I4:M6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="I7:M10"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="G10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -4736,50 +4736,50 @@
   <sheetData>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="40" t="s">
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="42"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="47"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="34"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="45"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="50"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="48"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="53"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
@@ -4842,18 +4842,18 @@
         <v>12</v>
       </c>
       <c r="C10" s="79"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="57"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="61"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="58"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="54"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="59"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="64" t="s">
@@ -5131,14 +5131,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B4:H6"/>
-    <mergeCell ref="I4:M6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="I7:M10"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="G10:H10"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
@@ -5151,6 +5143,14 @@
     <mergeCell ref="J11:J13"/>
     <mergeCell ref="K11:K13"/>
     <mergeCell ref="L11:L13"/>
+    <mergeCell ref="B4:H6"/>
+    <mergeCell ref="I4:M6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="I7:M10"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="G10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -5183,50 +5183,50 @@
   <sheetData>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="40" t="s">
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="42"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="47"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="34"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="45"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="50"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="48"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="53"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
@@ -5289,18 +5289,18 @@
         <v>12</v>
       </c>
       <c r="C10" s="79"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="57"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="61"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="58"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="54"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="59"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="64" t="s">
@@ -5578,14 +5578,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B4:H6"/>
-    <mergeCell ref="I4:M6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="I7:M10"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="G10:H10"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
@@ -5598,6 +5590,14 @@
     <mergeCell ref="J11:J13"/>
     <mergeCell ref="K11:K13"/>
     <mergeCell ref="L11:L13"/>
+    <mergeCell ref="B4:H6"/>
+    <mergeCell ref="I4:M6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="I7:M10"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="G10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -5629,50 +5629,50 @@
   <sheetData>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="40" t="s">
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="42"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="47"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="34"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="45"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="50"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="48"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="53"/>
     </row>
     <row r="7" spans="2:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
@@ -5735,18 +5735,18 @@
         <v>12</v>
       </c>
       <c r="C10" s="79"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="57"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="61"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="58"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="54"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="59"/>
     </row>
     <row r="11" spans="2:13" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="64" t="s">
@@ -5972,14 +5972,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B4:H6"/>
-    <mergeCell ref="I4:M6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="I7:M10"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="G10:H10"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
@@ -5992,6 +5984,14 @@
     <mergeCell ref="J11:J13"/>
     <mergeCell ref="K11:K13"/>
     <mergeCell ref="L11:L13"/>
+    <mergeCell ref="B4:H6"/>
+    <mergeCell ref="I4:M6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="I7:M10"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="G10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Se añade caso de prueba para CU4
</commit_message>
<xml_diff>
--- a/Documentos proyecto San Ambiente/Fase2/Casos de Prueba/Casos de prueba plantilla.xlsx
+++ b/Documentos proyecto San Ambiente/Fase2/Casos de Prueba/Casos de prueba plantilla.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SanAmbiente\Proyecto-Sanambiente\Documentos proyecto San Ambiente\Fase2\Casos de Prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BC60CD-8F24-46F7-A882-1F77E0548FA3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE99D36-73F0-4085-8AEC-5494E25FC802}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="CU5" sheetId="7" r:id="rId6"/>
     <sheet name="CU6" sheetId="8" r:id="rId7"/>
     <sheet name="CU11" sheetId="9" r:id="rId8"/>
+    <sheet name="CU4" sheetId="10" r:id="rId9"/>
+    <sheet name="CU1" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -38,6 +40,32 @@
   </authors>
   <commentList>
     <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">De acuerdo a los procesos  identificados en la 
+MDF
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Claudia Insuasty</author>
+  </authors>
+  <commentList>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{0B66682C-3B61-43D0-BB24-9FB701EB419B}">
       <text>
         <r>
           <rPr>
@@ -239,8 +267,34 @@
 </comments>
 </file>
 
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Claudia Insuasty</author>
+  </authors>
+  <commentList>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{44DDD929-CB83-4EE9-B109-8AB74F0B9D4A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">De acuerdo a los procesos  identificados en la 
+MDF
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="209">
   <si>
     <t>EJECUCION DE PRUEBAS</t>
   </si>
@@ -1627,6 +1681,163 @@
   </si>
   <si>
     <t>Se espera que el aplicativo internamente dentro del codigo realice la encriptacion del texto obtenido en el campo password, se realizara por el metodo SHA1 o el metodo de encryptacion MD5</t>
+  </si>
+  <si>
+    <t>CU4</t>
+  </si>
+  <si>
+    <t>Crear estacion (Tabla Parametro)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> crear Estacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario ingresará a la pantalla crear Estacion, el sistema deberá ingresar y cargar todo el contenido en un tiempo mínimo de 5 segundo. </t>
+  </si>
+  <si>
+    <t>Se dará click en el botón nuevo Estacion, se ingresará a la pantalla de crear Estacion y se tomará el tiempo en que el aplicativo da respuesta. Este tiempo debe ser mínimo 5 segundos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se espera que el aplicativo al ingresar en la pantalla de crear Estacion, el tiempo de repuesta sea inferior y como mínimo a 5 segundo, para ingresar y cargar su contenido. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id carga automáticamente tipo int
+Se ingresa nombre campo Estacion: Valores numéricos [0-9] (El sistema no debe permitir el ingreso)
+Se ingresan valores aleatorios tipo int mayor a 50 caracteres. (El sistema debe mostrar mensaje de validación) 
+Se ingresa nombre campo observacion: Esto es una prueba tipo String. 
+Se ingresan valores [a-z]  tipo String mayor a 50 caracteres. (El sistema debe mostrar mensaje de validación)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se probaran los metodos agregar Estacion
+</t>
+  </si>
+  <si>
+    <t>El ejecutar el test de la prueba unitari, debera mostrar en pantalla, la consultarealizada para la Estacion creada anteriormente</t>
+  </si>
+  <si>
+    <t>Se diligencias los campos nombre, nombre corto estacion,serial,observación, localización, latitud,longitud, elevación, el usuario oprime el botón guardar, el sistema deberá guardar la información en base de datos y mostrar mensaje de confirmación en pantalla.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario ingresará a la pantalla crear Estacion, el sistema cargará Id de la nueva Estacion a crear automáticamente, el usuario diligencia los campos nombre, nombre corto estacion,serial,observación, localización, latitud,longitud, elevación, los campos solo recibirán máximo 50 caracteres. </t>
+  </si>
+  <si>
+    <t>El usuario ingresará a la pantalla crear Estacion, el sistema cargará Id de la nueva Estacion a crear automáticamente, el usuario diligencia los campos nombre, nombre corto estacion,serial,observación, localización, latitud,longitud, elevación, los campos solo recibirán máximo 50 caracteres.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id carga automáticamente tipo int
+Se ingresa nombre campo Estacion:Chapinero  
+Se ingresan valores [a-z] tipo String min 50 caracteres.
+Se ingresa nombre campo nombre corto estacion: Chap
+Se ingresan valores [a-z] tipo String min 50 caracteres.
+Se ingresa nombre campo nombre corto: Chap
+Se ingresan valores [a-z] tipo String min 50 caracteres.
+Se ingresa campo serial: chapinero
+Se ingresan valores [a-z] tipo String min 50 caracteres.
+Se ingresa campo ,observación: Esto es una prueba.
+Se ingresan valores [a-z] tipo String min 50 caracteres.
+Se ingresa campo ,observación: Esto es una prueba.
+Se ingresan valores [a-z] tipo String min 50 caracteres.
+Se ingresa campo , localización: Ubicada al centro de la ciudad.
+Se ingresan valores [a-z] tipo String min 50 caracteres.
+Se ingresa campo , latitud: Ubicada al centro de la ciudad.
+Se ingresan valores [a-z] tipo String min 50 caracteres.
+Se ingresa campo , longitud: Ubicada al centro de la ciudad.
+Se ingresan valores [a-z] tipo String min 50 caracteres.
+Se ingresa campo , elevacion: Ubicada al centro de la ciudad.
+Se ingresan valores [a-z] tipo String min 50 caracteres.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campos nombre, nombre corto estacion,serial,observación, localización, latitud,longitud, elevació
+</t>
+  </si>
+  <si>
+    <t>Se diligencia le campo nombre: Estacion estacion
+nombre, nombre corto estacion,serial,observación, localización, latitud,longitud, elevació.</t>
+  </si>
+  <si>
+    <r>
+      <t>agregarEstacion(id_estacion, nombre_estacion, nombre_corto_estacion, serial_estacion, organización_estacion, categoría_estacion, base_tiempo_estacion, observación_estacion, región_estacion, ciudad_estacion, localización_estacion, latitud_estacion, longitud_estacion, elevación_estacion, gmt_estacion, protocolo_estacion), se escribira prueba unitaria donde:
+id_estacion:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+nombre_estacion:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Estacion</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Prueba
+nombre_corto_estacion:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Est.Prue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>consultarEstacion(id_estacion, nombre_estacion, nombre_corto_estacion, serial_estacion, ciudad_estacion, protocolo_estacion), se escribira prueba unitaria donde:
+id_estacion:1 
+se debera cargar la informacion asociada a este id</t>
+  </si>
+  <si>
+    <t>Conectar con estacion</t>
+  </si>
+  <si>
+    <t>CU1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conectar con estacion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario ingresará a la pantalla conectar con estacion, el sistema deberá ingresar y cargar todo el contenido en un tiempo mínimo de 5 segundo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> se ingresará a la pantalla de conectar con estacion y se tomará el tiempo en que el aplicativo da respuesta. Este tiempo debe ser mínimo 5 segundos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se espera que el aplicativo al ingresar en la pantalla de conectar con estacion, el tiempo de repuesta sea inferior y como mínimo a 5 segundo, para ingresar y cargar su contenido. </t>
   </si>
 </sst>
 </file>
@@ -2019,7 +2230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2112,6 +2323,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2255,6 +2472,123 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2560,214 +2894,214 @@
   <sheetData>
     <row r="5" spans="2:13" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="45" t="s">
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="47"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="49"/>
     </row>
     <row r="7" spans="2:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="39"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="50"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="52"/>
     </row>
     <row r="8" spans="2:13" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="42"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="53"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="55"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="31" t="s">
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="57"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
     </row>
     <row r="12" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
     </row>
     <row r="13" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
     </row>
     <row r="14" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="61"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="63"/>
       <c r="F14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="62"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="33"/>
     </row>
     <row r="15" spans="2:13" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="35" t="s">
+      <c r="F15" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="35" t="s">
+      <c r="G15" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="H15" s="35" t="s">
+      <c r="H15" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="I15" s="31" t="s">
+      <c r="I15" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="J15" s="31" t="s">
+      <c r="J15" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="K15" s="31" t="s">
+      <c r="K15" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="L15" s="31" t="s">
+      <c r="L15" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="31" t="s">
+      <c r="M15" s="33" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
     </row>
     <row r="17" spans="2:13" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
@@ -2924,12 +3258,379 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC56C1B5-61AC-414C-89B9-0AFDA14EAE32}">
+  <dimension ref="C3:N21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="5" customWidth="1"/>
+    <col min="11" max="11" width="4.42578125" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" customWidth="1"/>
+    <col min="13" max="13" width="5.28515625" customWidth="1"/>
+    <col min="14" max="14" width="4.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C4" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="49"/>
+    </row>
+    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="52"/>
+    </row>
+    <row r="6" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="44"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="55"/>
+    </row>
+    <row r="7" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="75" t="s">
+        <v>204</v>
+      </c>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="69" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="70"/>
+      <c r="N7" s="71"/>
+    </row>
+    <row r="8" spans="3:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="78" t="s">
+        <v>203</v>
+      </c>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="73"/>
+      <c r="N8" s="74"/>
+    </row>
+    <row r="9" spans="3:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="78" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="74"/>
+    </row>
+    <row r="10" spans="3:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="81"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="64"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="60"/>
+      <c r="N10" s="61"/>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C11" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="66" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="66" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="N11" s="66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="67"/>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="68"/>
+      <c r="N13" s="68"/>
+    </row>
+    <row r="14" spans="3:14" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="I14" s="8"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+    </row>
+    <row r="15" spans="3:14" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="C15" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="E15" s="29"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C16" s="24"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C17" s="24"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C18" s="24"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C19" s="24"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+    </row>
+    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C20" s="24"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+    </row>
+    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C21" s="24"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="L11:L13"/>
+    <mergeCell ref="M11:M13"/>
+    <mergeCell ref="N11:N13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="C4:I6"/>
+    <mergeCell ref="J4:N6"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="J7:N10"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="H10:I10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:M21"/>
   <sheetViews>
     <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B14" sqref="B14:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2950,190 +3651,190 @@
   <sheetData>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="45" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="47"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="49"/>
     </row>
     <row r="5" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="50"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="52"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="42"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="53"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="55"/>
     </row>
     <row r="7" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="67" t="s">
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="69"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="71"/>
     </row>
     <row r="8" spans="2:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="76" t="s">
+      <c r="C8" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="72"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="74"/>
     </row>
     <row r="9" spans="2:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="76" t="s">
+      <c r="C9" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="71"/>
-      <c r="L9" s="71"/>
-      <c r="M9" s="72"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="74"/>
     </row>
     <row r="10" spans="2:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="79"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="61"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="63"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="62"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="59"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="61"/>
     </row>
     <row r="11" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="64" t="s">
+      <c r="E11" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="64" t="s">
+      <c r="F11" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="64" t="s">
+      <c r="G11" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="64" t="s">
+      <c r="H11" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="64" t="s">
+      <c r="I11" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="64" t="s">
+      <c r="J11" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="64" t="s">
+      <c r="K11" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="64" t="s">
+      <c r="L11" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="64" t="s">
+      <c r="M11" s="66" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="65"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="65"/>
-      <c r="M12" s="65"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
     </row>
     <row r="13" spans="2:13" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="66"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="68"/>
     </row>
     <row r="14" spans="2:13" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
@@ -3376,7 +4077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B16777-4111-4BC8-A284-35AF9BE8FDAD}">
   <dimension ref="B3:M21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <selection activeCell="C9" sqref="C9:H9"/>
     </sheetView>
   </sheetViews>
@@ -3398,190 +4099,190 @@
   <sheetData>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="45" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="47"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="49"/>
     </row>
     <row r="5" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="50"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="52"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="42"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="53"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="55"/>
     </row>
     <row r="7" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="75" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="67" t="s">
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="69"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="71"/>
     </row>
     <row r="8" spans="2:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="76" t="s">
+      <c r="C8" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="72"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="74"/>
     </row>
     <row r="9" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="76" t="s">
+      <c r="C9" s="78" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="71"/>
-      <c r="L9" s="71"/>
-      <c r="M9" s="72"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="74"/>
     </row>
     <row r="10" spans="2:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="79"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="61"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="63"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="62"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="59"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="61"/>
     </row>
     <row r="11" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="64" t="s">
+      <c r="E11" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="64" t="s">
+      <c r="F11" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="64" t="s">
+      <c r="G11" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="64" t="s">
+      <c r="H11" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="64" t="s">
+      <c r="I11" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="64" t="s">
+      <c r="J11" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="64" t="s">
+      <c r="K11" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="64" t="s">
+      <c r="L11" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="64" t="s">
+      <c r="M11" s="66" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="65"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="65"/>
-      <c r="M12" s="65"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
     </row>
     <row r="13" spans="2:13" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="66"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="68"/>
     </row>
     <row r="14" spans="2:13" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
@@ -3823,8 +4524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF69378-5C9E-410A-9F24-6A5C43D39D40}">
   <dimension ref="B3:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:H7"/>
+    <sheetView zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3844,190 +4545,190 @@
   <sheetData>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="45" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="47"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="49"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="50"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="52"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="42"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="53"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="55"/>
     </row>
     <row r="7" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="75" t="s">
         <v>79</v>
       </c>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="67" t="s">
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="69"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="71"/>
     </row>
     <row r="8" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="76" t="s">
+      <c r="C8" s="78" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="72"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="74"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="76" t="s">
+      <c r="C9" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="71"/>
-      <c r="L9" s="71"/>
-      <c r="M9" s="72"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="74"/>
     </row>
     <row r="10" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="79"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="61"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="63"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="62"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="59"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="61"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="64" t="s">
+      <c r="E11" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="64" t="s">
+      <c r="F11" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="64" t="s">
+      <c r="G11" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="64" t="s">
+      <c r="H11" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="64" t="s">
+      <c r="I11" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="64" t="s">
+      <c r="J11" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="64" t="s">
+      <c r="K11" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="64" t="s">
+      <c r="L11" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="64" t="s">
+      <c r="M11" s="66" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="65"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="65"/>
-      <c r="M12" s="65"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
     </row>
     <row r="13" spans="2:13" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="66"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="68"/>
     </row>
     <row r="14" spans="2:13" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="24" t="s">
@@ -4290,190 +4991,190 @@
   <sheetData>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="45" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="47"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="49"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="50"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="52"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="42"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="53"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="55"/>
     </row>
     <row r="7" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="75" t="s">
         <v>122</v>
       </c>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="67" t="s">
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="69"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="71"/>
     </row>
     <row r="8" spans="2:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="76" t="s">
+      <c r="C8" s="78" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="72"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="74"/>
     </row>
     <row r="9" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="76" t="s">
+      <c r="C9" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="71"/>
-      <c r="L9" s="71"/>
-      <c r="M9" s="72"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="74"/>
     </row>
     <row r="10" spans="2:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="79"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="61"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="63"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="62"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="59"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="61"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="64" t="s">
+      <c r="E11" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="64" t="s">
+      <c r="F11" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="64" t="s">
+      <c r="G11" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="64" t="s">
+      <c r="H11" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="64" t="s">
+      <c r="I11" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="64" t="s">
+      <c r="J11" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="64" t="s">
+      <c r="K11" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="64" t="s">
+      <c r="L11" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="64" t="s">
+      <c r="M11" s="66" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="65"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="65"/>
-      <c r="M12" s="65"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
     </row>
     <row r="13" spans="2:13" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="66"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="68"/>
     </row>
     <row r="14" spans="2:13" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
@@ -4715,7 +5416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B83024-9021-43CC-86C0-CBE472185E4B}">
   <dimension ref="B3:M21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <selection activeCell="C9" sqref="C9:H9"/>
     </sheetView>
   </sheetViews>
@@ -4736,190 +5437,190 @@
   <sheetData>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="45" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="47"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="49"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="50"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="52"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="42"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="53"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="55"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="75" t="s">
         <v>123</v>
       </c>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="67" t="s">
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="69"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="71"/>
     </row>
     <row r="8" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="76" t="s">
+      <c r="C8" s="78" t="s">
         <v>124</v>
       </c>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="72"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="74"/>
     </row>
     <row r="9" spans="2:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="76" t="s">
+      <c r="C9" s="78" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="71"/>
-      <c r="L9" s="71"/>
-      <c r="M9" s="72"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="74"/>
     </row>
     <row r="10" spans="2:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="79"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="61"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="63"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="62"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="59"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="61"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="64" t="s">
+      <c r="E11" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="64" t="s">
+      <c r="F11" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="64" t="s">
+      <c r="G11" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="64" t="s">
+      <c r="H11" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="64" t="s">
+      <c r="I11" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="64" t="s">
+      <c r="J11" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="64" t="s">
+      <c r="K11" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="64" t="s">
+      <c r="L11" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="64" t="s">
+      <c r="M11" s="66" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="65"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="65"/>
-      <c r="M12" s="65"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
     </row>
     <row r="13" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="66"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="68"/>
     </row>
     <row r="14" spans="2:13" ht="168" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
@@ -5183,190 +5884,190 @@
   <sheetData>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="45" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="47"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="49"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="50"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="52"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="42"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="53"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="55"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="75" t="s">
         <v>157</v>
       </c>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="67" t="s">
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="69"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="71"/>
     </row>
     <row r="8" spans="2:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="76" t="s">
+      <c r="C8" s="78" t="s">
         <v>143</v>
       </c>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="72"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="74"/>
     </row>
     <row r="9" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="76" t="s">
+      <c r="C9" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="71"/>
-      <c r="L9" s="71"/>
-      <c r="M9" s="72"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="74"/>
     </row>
     <row r="10" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="79"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="61"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="63"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="62"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="59"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="61"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="64" t="s">
+      <c r="E11" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="64" t="s">
+      <c r="F11" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="64" t="s">
+      <c r="G11" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="64" t="s">
+      <c r="H11" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="64" t="s">
+      <c r="I11" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="64" t="s">
+      <c r="J11" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="64" t="s">
+      <c r="K11" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="64" t="s">
+      <c r="L11" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="64" t="s">
+      <c r="M11" s="66" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="65"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="65"/>
-      <c r="M12" s="65"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
     </row>
     <row r="13" spans="2:13" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="66"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="68"/>
     </row>
     <row r="14" spans="2:13" ht="201" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
@@ -5608,8 +6309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74ED4A39-E2C2-40A4-A2EF-E325FC0589EC}">
   <dimension ref="B3:M19"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="A7" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5629,192 +6330,192 @@
   <sheetData>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="45" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="47"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="49"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="50"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="52"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="42"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="53"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="55"/>
     </row>
     <row r="7" spans="2:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="75" t="s">
         <v>165</v>
       </c>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="67" t="s">
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="69"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="71"/>
     </row>
     <row r="8" spans="2:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="76" t="s">
+      <c r="C8" s="78" t="s">
         <v>166</v>
       </c>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="72"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="74"/>
     </row>
     <row r="9" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="76" t="s">
+      <c r="C9" s="78" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="71"/>
-      <c r="L9" s="71"/>
-      <c r="M9" s="72"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="74"/>
     </row>
     <row r="10" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="79"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="61"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="63"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="62"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="59"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="61"/>
     </row>
     <row r="11" spans="2:13" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="64" t="s">
+      <c r="E11" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="64" t="s">
+      <c r="F11" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="64" t="s">
+      <c r="G11" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="64" t="s">
+      <c r="H11" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="64" t="s">
+      <c r="I11" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="64" t="s">
+      <c r="J11" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="64" t="s">
+      <c r="K11" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="64" t="s">
+      <c r="L11" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="64" t="s">
+      <c r="M11" s="66" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="65"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="65"/>
-      <c r="M12" s="65"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
     </row>
     <row r="13" spans="2:13" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="66"/>
-    </row>
-    <row r="14" spans="2:13" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="68"/>
+    </row>
+    <row r="14" spans="2:13" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
         <v>24</v>
       </c>
@@ -5996,4 +6697,429 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BEA60B5-646D-4C1D-80DD-E023A21A3604}">
+  <dimension ref="B3:M21"/>
+  <sheetViews>
+    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="8" max="8" width="23" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" customWidth="1"/>
+    <col min="10" max="10" width="6" customWidth="1"/>
+    <col min="11" max="12" width="5.42578125" customWidth="1"/>
+    <col min="13" max="13" width="5.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="94" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="95"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="95"/>
+      <c r="M4" s="96"/>
+    </row>
+    <row r="5" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="88"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="99"/>
+    </row>
+    <row r="6" spans="2:13" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="91"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="93"/>
+      <c r="I6" s="100"/>
+      <c r="J6" s="101"/>
+      <c r="K6" s="101"/>
+      <c r="L6" s="101"/>
+      <c r="M6" s="102"/>
+    </row>
+    <row r="7" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="103" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7" s="104"/>
+      <c r="E7" s="104"/>
+      <c r="F7" s="104"/>
+      <c r="G7" s="104"/>
+      <c r="H7" s="105"/>
+      <c r="I7" s="106" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="107"/>
+      <c r="K7" s="107"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="108"/>
+    </row>
+    <row r="8" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="115" t="s">
+        <v>187</v>
+      </c>
+      <c r="D8" s="116"/>
+      <c r="E8" s="116"/>
+      <c r="F8" s="116"/>
+      <c r="G8" s="116"/>
+      <c r="H8" s="117"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="110"/>
+      <c r="K8" s="110"/>
+      <c r="L8" s="110"/>
+      <c r="M8" s="111"/>
+    </row>
+    <row r="9" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="115" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="116"/>
+      <c r="E9" s="116"/>
+      <c r="F9" s="116"/>
+      <c r="G9" s="116"/>
+      <c r="H9" s="117"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="110"/>
+      <c r="K9" s="110"/>
+      <c r="L9" s="110"/>
+      <c r="M9" s="111"/>
+    </row>
+    <row r="10" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="115"/>
+      <c r="D10" s="116"/>
+      <c r="E10" s="117"/>
+      <c r="F10" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="115"/>
+      <c r="H10" s="117"/>
+      <c r="I10" s="112"/>
+      <c r="J10" s="113"/>
+      <c r="K10" s="113"/>
+      <c r="L10" s="113"/>
+      <c r="M10" s="114"/>
+    </row>
+    <row r="11" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="82" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="82" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="82" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="82" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="82" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="82" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="82" t="s">
+        <v>8</v>
+      </c>
+      <c r="M11" s="82" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="0.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="83"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="83"/>
+      <c r="H12" s="83"/>
+      <c r="I12" s="83"/>
+      <c r="J12" s="83"/>
+      <c r="K12" s="83"/>
+      <c r="L12" s="83"/>
+      <c r="M12" s="83"/>
+    </row>
+    <row r="13" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="84"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="84"/>
+      <c r="F13" s="84"/>
+      <c r="G13" s="84"/>
+      <c r="H13" s="84"/>
+      <c r="I13" s="84"/>
+      <c r="J13" s="84"/>
+      <c r="K13" s="84"/>
+      <c r="L13" s="84"/>
+      <c r="M13" s="84"/>
+    </row>
+    <row r="14" spans="2:13" ht="203.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="H14" s="27"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+    </row>
+    <row r="15" spans="2:13" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="E15" s="119" t="s">
+        <v>198</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="27"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+    </row>
+    <row r="16" spans="2:13" ht="323.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="24"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="118"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+    </row>
+    <row r="17" spans="2:13" ht="242.25" x14ac:dyDescent="0.25">
+      <c r="B17" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="27"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+    </row>
+    <row r="18" spans="2:13" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="27"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+    </row>
+    <row r="19" spans="2:13" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="E19" s="119" t="s">
+        <v>201</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="27"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+    </row>
+    <row r="20" spans="2:13" ht="174" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="24"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="120"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+    </row>
+    <row r="21" spans="2:13" ht="210" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="H21" s="27"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="B4:H6"/>
+    <mergeCell ref="I4:M6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="I7:M10"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="M11:M13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="L11:L13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>